<commit_message>
feat: Partner with new structure for upload
</commit_message>
<xml_diff>
--- a/CONTACTOS-LA-INTEGRAL.xlsx
+++ b/CONTACTOS-LA-INTEGRAL.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">domicilio</t>
   </si>
   <si>
-    <t xml:space="preserve">María Modificada</t>
+    <t xml:space="preserve">Sin modificar a Marías</t>
   </si>
   <si>
     <t xml:space="preserve">González</t>
@@ -226,6 +226,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -247,11 +248,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -296,20 +299,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,307 +446,307 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>